<commit_message>
PROS-13075 - CCRU - POS 2020 KPIs - copy to SAND
</commit_message>
<xml_diff>
--- a/Projects/CCRU_SAND/Data/KPIs_2019/PoS 2019 - IC Cinema - CAP.xlsx
+++ b/Projects/CCRU_SAND/Data/KPIs_2019/PoS 2019 - IC Cinema - CAP.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\My folder\RED\POS 2019\POS_2019-12-16\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\My folder\RED\POS 2019\POS_2019-12-24\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46448CA0-8974-45E8-BBFF-6147AD204223}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1660681-E781-41E5-9C2B-CD6DB3BBA05C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection lockWindows="1"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="602" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="1200" windowWidth="21840" windowHeight="13140" tabRatio="602" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cinema" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <definedName name="_FilterDatabase_0" localSheetId="0">Cinema!$A$1:$AO$54</definedName>
     <definedName name="_FilterDatabase_0_0" localSheetId="0">Cinema!$A$1:$AO$54</definedName>
   </definedNames>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2760" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="690" uniqueCount="248">
   <si>
     <t>Sorting</t>
   </si>
@@ -625,9 +625,6 @@
     <t>AND</t>
   </si>
   <si>
-    <t>Menu Board, Cash Zone, SS_Cash Zone - Canteen, QSR, SS_Menu Board - Canteen, QSR</t>
-  </si>
-  <si>
     <t>35
 36</t>
   </si>
@@ -819,10 +816,7 @@
     <t>Cash Zone; SS_Cash Zone - Canteen, QSR; Promo SSD Display IC</t>
   </si>
   <si>
-    <t>Menu Board; Cash Zone; SS_Cash Zone - Canteen, QSR, SS_Menu Board - Canteen, QSR</t>
-  </si>
-  <si>
-    <t>Menu Board; Cash Zone; SS_Cash Zone - Canteen, QSR; SS_Menu Board - Canteen, QSR</t>
+    <t>Combo1; Combo2; Combo3; Menu Board; Cash Zone; SS_Cash Zone - Canteen, QSR; SS_Menu Board - Canteen, QSR</t>
   </si>
 </sst>
 </file>
@@ -1346,10 +1340,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMK54"/>
   <sheetViews>
-    <sheetView windowProtection="1" tabSelected="1" topLeftCell="S1" zoomScale="65" zoomScaleNormal="65" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView windowProtection="1" tabSelected="1" zoomScale="65" zoomScaleNormal="65" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="V1" sqref="V1"/>
-      <selection pane="bottomLeft" activeCell="Z49" sqref="Z49"/>
+      <selection pane="bottomLeft" activeCell="Z41" sqref="Z41:Z47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1715,7 +1709,7 @@
       <c r="Y4" s="6"/>
       <c r="Z4" s="14"/>
       <c r="AA4" s="6" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="AB4" s="6"/>
       <c r="AC4" s="6"/>
@@ -1798,7 +1792,7 @@
       <c r="Y5" s="6"/>
       <c r="Z5" s="14"/>
       <c r="AA5" s="6" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="AB5" s="6"/>
       <c r="AC5" s="6"/>
@@ -1881,7 +1875,7 @@
       <c r="Y6" s="6"/>
       <c r="Z6" s="14"/>
       <c r="AA6" s="6" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="AB6" s="6"/>
       <c r="AC6" s="6"/>
@@ -1964,7 +1958,7 @@
       <c r="Y7" s="6"/>
       <c r="Z7" s="14"/>
       <c r="AA7" s="6" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="AB7" s="6"/>
       <c r="AC7" s="6"/>
@@ -2047,7 +2041,7 @@
       <c r="Y8" s="6"/>
       <c r="Z8" s="14"/>
       <c r="AA8" s="6" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="AB8" s="6"/>
       <c r="AC8" s="6"/>
@@ -2130,7 +2124,7 @@
       <c r="Y9" s="6"/>
       <c r="Z9" s="14"/>
       <c r="AA9" s="6" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="AB9" s="6"/>
       <c r="AC9" s="6"/>
@@ -2213,7 +2207,7 @@
       <c r="Y10" s="6"/>
       <c r="Z10" s="14"/>
       <c r="AA10" s="6" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="AB10" s="6"/>
       <c r="AC10" s="6"/>
@@ -2296,7 +2290,7 @@
       <c r="Y11" s="6"/>
       <c r="Z11" s="14"/>
       <c r="AA11" s="6" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="AB11" s="6"/>
       <c r="AC11" s="6"/>
@@ -2452,7 +2446,7 @@
       <c r="Y13" s="6"/>
       <c r="Z13" s="14"/>
       <c r="AA13" s="6" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="AB13" s="6"/>
       <c r="AC13" s="6"/>
@@ -2535,7 +2529,7 @@
       <c r="Y14" s="6"/>
       <c r="Z14" s="14"/>
       <c r="AA14" s="6" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="AB14" s="6"/>
       <c r="AC14" s="6"/>
@@ -2691,7 +2685,7 @@
       <c r="Y16" s="6"/>
       <c r="Z16" s="14"/>
       <c r="AA16" s="6" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="AB16" s="6"/>
       <c r="AC16" s="6"/>
@@ -2847,7 +2841,7 @@
       <c r="Y18" s="6"/>
       <c r="Z18" s="14"/>
       <c r="AA18" s="6" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="AB18" s="6"/>
       <c r="AC18" s="6"/>
@@ -2930,7 +2924,7 @@
       <c r="Y19" s="6"/>
       <c r="Z19" s="14"/>
       <c r="AA19" s="6" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="AB19" s="6"/>
       <c r="AC19" s="6"/>
@@ -3013,7 +3007,7 @@
       <c r="Y20" s="6"/>
       <c r="Z20" s="14"/>
       <c r="AA20" s="6" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="AB20" s="6"/>
       <c r="AC20" s="6"/>
@@ -3096,7 +3090,7 @@
       <c r="Y21" s="6"/>
       <c r="Z21" s="14"/>
       <c r="AA21" s="6" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="AB21" s="6"/>
       <c r="AC21" s="6"/>
@@ -3252,7 +3246,7 @@
       <c r="Y23" s="6"/>
       <c r="Z23" s="14"/>
       <c r="AA23" s="6" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="AB23" s="6"/>
       <c r="AC23" s="6"/>
@@ -3335,7 +3329,7 @@
       <c r="Y24" s="6"/>
       <c r="Z24" s="14"/>
       <c r="AA24" s="6" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="AB24" s="6"/>
       <c r="AC24" s="6"/>
@@ -3418,7 +3412,7 @@
       <c r="Y25" s="6"/>
       <c r="Z25" s="14"/>
       <c r="AA25" s="6" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="AB25" s="6"/>
       <c r="AC25" s="6"/>
@@ -3501,7 +3495,7 @@
       <c r="Y26" s="6"/>
       <c r="Z26" s="14"/>
       <c r="AA26" s="6" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="AB26" s="6"/>
       <c r="AC26" s="6"/>
@@ -3584,7 +3578,7 @@
       <c r="Y27" s="6"/>
       <c r="Z27" s="14"/>
       <c r="AA27" s="6" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="AB27" s="6"/>
       <c r="AC27" s="6"/>
@@ -3667,7 +3661,7 @@
       <c r="Y28" s="6"/>
       <c r="Z28" s="14"/>
       <c r="AA28" s="6" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="AB28" s="6"/>
       <c r="AC28" s="6"/>
@@ -3750,7 +3744,7 @@
       <c r="Y29" s="6"/>
       <c r="Z29" s="14"/>
       <c r="AA29" s="6" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="AB29" s="6"/>
       <c r="AC29" s="6"/>
@@ -4256,7 +4250,7 @@
       <c r="X36" s="6"/>
       <c r="Y36" s="6"/>
       <c r="Z36" s="14" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="AA36" s="6"/>
       <c r="AB36" s="6"/>
@@ -4578,7 +4572,7 @@
       <c r="X40" s="6"/>
       <c r="Y40" s="6"/>
       <c r="Z40" s="15" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="AA40" s="6"/>
       <c r="AB40" s="6"/>
@@ -4655,7 +4649,7 @@
       <c r="X41" s="6"/>
       <c r="Y41" s="6"/>
       <c r="Z41" s="14" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="AA41" s="6"/>
       <c r="AB41" s="6"/>
@@ -4681,7 +4675,7 @@
         <v>34</v>
       </c>
       <c r="AN41" s="9" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="AO41" s="6">
         <v>400</v>
@@ -4704,10 +4698,10 @@
         <v>182</v>
       </c>
       <c r="F42" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="G42" s="6" t="s">
         <v>189</v>
-      </c>
-      <c r="G42" s="6" t="s">
-        <v>190</v>
       </c>
       <c r="H42" s="6" t="s">
         <v>56</v>
@@ -4721,10 +4715,10 @@
       <c r="M42" s="6"/>
       <c r="N42" s="6"/>
       <c r="O42" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="P42" s="11" t="s">
         <v>191</v>
-      </c>
-      <c r="P42" s="11" t="s">
-        <v>192</v>
       </c>
       <c r="Q42" s="6"/>
       <c r="R42" s="6"/>
@@ -4740,7 +4734,7 @@
       <c r="X42" s="6"/>
       <c r="Y42" s="6"/>
       <c r="Z42" s="14" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="AA42" s="6"/>
       <c r="AB42" s="6"/>
@@ -4785,10 +4779,10 @@
         <v>182</v>
       </c>
       <c r="F43" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="G43" s="6" t="s">
         <v>193</v>
-      </c>
-      <c r="G43" s="6" t="s">
-        <v>194</v>
       </c>
       <c r="H43" s="12" t="s">
         <v>56</v>
@@ -4802,13 +4796,13 @@
       <c r="M43" s="6"/>
       <c r="N43" s="6"/>
       <c r="O43" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="P43" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="P43" s="7" t="s">
+      <c r="Q43" s="6" t="s">
         <v>196</v>
-      </c>
-      <c r="Q43" s="6" t="s">
-        <v>197</v>
       </c>
       <c r="R43" s="6"/>
       <c r="S43" s="6" t="s">
@@ -4823,7 +4817,7 @@
       <c r="X43" s="6"/>
       <c r="Y43" s="6"/>
       <c r="Z43" s="14" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="AA43" s="6"/>
       <c r="AB43" s="6"/>
@@ -4839,7 +4833,7 @@
       <c r="AH43" s="6"/>
       <c r="AI43" s="6"/>
       <c r="AJ43" s="6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="AK43" s="6"/>
       <c r="AL43" s="6">
@@ -4867,13 +4861,13 @@
         <v>43</v>
       </c>
       <c r="E44" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="F44" s="6" t="s">
         <v>199</v>
       </c>
-      <c r="F44" s="6" t="s">
+      <c r="G44" s="6" t="s">
         <v>200</v>
-      </c>
-      <c r="G44" s="6" t="s">
-        <v>201</v>
       </c>
       <c r="H44" s="12" t="s">
         <v>185</v>
@@ -4900,7 +4894,7 @@
       <c r="X44" s="6"/>
       <c r="Y44" s="6"/>
       <c r="Z44" s="14" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="AA44" s="6"/>
       <c r="AB44" s="6"/>
@@ -4947,13 +4941,13 @@
         <v>182</v>
       </c>
       <c r="F45" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="G45" s="6" t="s">
         <v>202</v>
       </c>
-      <c r="G45" s="6" t="s">
+      <c r="H45" s="6" t="s">
         <v>203</v>
-      </c>
-      <c r="H45" s="6" t="s">
-        <v>204</v>
       </c>
       <c r="I45" s="6"/>
       <c r="J45" s="6"/>
@@ -4977,7 +4971,7 @@
       <c r="X45" s="6"/>
       <c r="Y45" s="6"/>
       <c r="Z45" s="14" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="AA45" s="6"/>
       <c r="AB45" s="6"/>
@@ -5001,7 +4995,7 @@
         <v>769</v>
       </c>
       <c r="AN45" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="AO45" s="6">
         <v>680</v>
@@ -5024,10 +5018,10 @@
         <v>182</v>
       </c>
       <c r="F46" s="12" t="s">
+        <v>205</v>
+      </c>
+      <c r="G46" s="6" t="s">
         <v>206</v>
-      </c>
-      <c r="G46" s="6" t="s">
-        <v>207</v>
       </c>
       <c r="H46" s="6" t="s">
         <v>56</v>
@@ -5041,22 +5035,22 @@
       <c r="M46" s="6"/>
       <c r="N46" s="6"/>
       <c r="O46" s="6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="P46" s="6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="Q46" s="12" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="R46" s="6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="S46" s="6" t="s">
         <v>57</v>
       </c>
       <c r="T46" s="6" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="U46" s="6"/>
       <c r="V46" s="6"/>
@@ -5064,7 +5058,7 @@
       <c r="X46" s="6"/>
       <c r="Y46" s="6"/>
       <c r="Z46" s="14" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="AA46" s="6"/>
       <c r="AB46" s="6"/>
@@ -5109,10 +5103,10 @@
         <v>182</v>
       </c>
       <c r="F47" s="12" t="s">
+        <v>209</v>
+      </c>
+      <c r="G47" s="6" t="s">
         <v>210</v>
-      </c>
-      <c r="G47" s="6" t="s">
-        <v>211</v>
       </c>
       <c r="H47" s="12" t="s">
         <v>56</v>
@@ -5126,13 +5120,13 @@
       <c r="M47" s="6"/>
       <c r="N47" s="6"/>
       <c r="O47" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="P47" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="P47" s="7" t="s">
+      <c r="Q47" s="6" t="s">
         <v>196</v>
-      </c>
-      <c r="Q47" s="6" t="s">
-        <v>197</v>
       </c>
       <c r="R47" s="6"/>
       <c r="S47" s="6" t="s">
@@ -5147,7 +5141,7 @@
       <c r="X47" s="6"/>
       <c r="Y47" s="6"/>
       <c r="Z47" s="14" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="AA47" s="6"/>
       <c r="AB47" s="6"/>
@@ -5163,7 +5157,7 @@
       <c r="AH47" s="6"/>
       <c r="AI47" s="6"/>
       <c r="AJ47" s="6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="AK47" s="6"/>
       <c r="AL47" s="6">
@@ -5188,24 +5182,24 @@
         <v>42</v>
       </c>
       <c r="D48" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="E48" s="6" t="s">
         <v>212</v>
       </c>
-      <c r="E48" s="6" t="s">
+      <c r="F48" s="6" t="s">
         <v>213</v>
       </c>
-      <c r="F48" s="6" t="s">
+      <c r="G48" s="6" t="s">
         <v>214</v>
       </c>
-      <c r="G48" s="6" t="s">
+      <c r="H48" s="6" t="s">
         <v>215</v>
-      </c>
-      <c r="H48" s="6" t="s">
-        <v>216</v>
       </c>
       <c r="I48" s="6"/>
       <c r="J48" s="6"/>
       <c r="K48" s="6" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="L48" s="6"/>
       <c r="M48" s="6"/>
@@ -5216,7 +5210,7 @@
       <c r="R48" s="6"/>
       <c r="S48" s="6"/>
       <c r="T48" s="6" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="U48" s="6"/>
       <c r="V48" s="6"/>
@@ -5255,37 +5249,37 @@
         <v>42</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E49" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="F49" s="6" t="s">
         <v>219</v>
       </c>
-      <c r="F49" s="6" t="s">
+      <c r="G49" s="6" t="s">
         <v>220</v>
       </c>
-      <c r="G49" s="6" t="s">
+      <c r="H49" s="6" t="s">
         <v>221</v>
-      </c>
-      <c r="H49" s="6" t="s">
-        <v>222</v>
       </c>
       <c r="I49" s="6"/>
       <c r="J49" s="6"/>
       <c r="K49" s="6" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="L49" s="6"/>
       <c r="M49" s="6"/>
       <c r="N49" s="6"/>
       <c r="O49" s="6"/>
       <c r="P49" s="9" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="Q49" s="6"/>
       <c r="R49" s="6"/>
       <c r="S49" s="6"/>
       <c r="T49" s="6" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="U49" s="6"/>
       <c r="V49" s="6"/>
@@ -5324,37 +5318,37 @@
         <v>42</v>
       </c>
       <c r="D50" s="6" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E50" s="6" t="s">
         <v>179</v>
       </c>
       <c r="F50" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="G50" s="6" t="s">
         <v>225</v>
       </c>
-      <c r="G50" s="6" t="s">
-        <v>226</v>
-      </c>
       <c r="H50" s="6" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="I50" s="6"/>
       <c r="J50" s="6"/>
       <c r="K50" s="6" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="L50" s="6"/>
       <c r="M50" s="6"/>
       <c r="N50" s="6"/>
       <c r="O50" s="6"/>
       <c r="P50" s="9" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="Q50" s="6"/>
       <c r="R50" s="6"/>
       <c r="S50" s="6"/>
       <c r="T50" s="6" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="U50" s="6"/>
       <c r="V50" s="6"/>
@@ -5393,39 +5387,39 @@
         <v>42</v>
       </c>
       <c r="D51" s="6" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E51" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="F51" s="6" t="s">
         <v>228</v>
       </c>
-      <c r="F51" s="6" t="s">
-        <v>229</v>
-      </c>
       <c r="G51" s="6" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="H51" s="6" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="I51" s="6"/>
       <c r="J51" s="6"/>
       <c r="K51" s="6" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="L51" s="6"/>
       <c r="M51" s="6"/>
       <c r="N51" s="6"/>
       <c r="O51" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="P51" s="9" t="s">
         <v>230</v>
-      </c>
-      <c r="P51" s="9" t="s">
-        <v>231</v>
       </c>
       <c r="Q51" s="6"/>
       <c r="R51" s="6"/>
       <c r="S51" s="6"/>
       <c r="T51" s="6" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="U51" s="6"/>
       <c r="V51" s="6"/>
@@ -5464,39 +5458,39 @@
         <v>42</v>
       </c>
       <c r="D52" s="6" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E52" s="6" t="s">
         <v>182</v>
       </c>
       <c r="F52" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="G52" s="6" t="s">
         <v>232</v>
       </c>
-      <c r="G52" s="6" t="s">
-        <v>233</v>
-      </c>
       <c r="H52" s="6" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="I52" s="6"/>
       <c r="J52" s="6"/>
       <c r="K52" s="6" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="L52" s="6"/>
       <c r="M52" s="6"/>
       <c r="N52" s="6"/>
       <c r="O52" s="6" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="P52" s="9" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="Q52" s="6"/>
       <c r="R52" s="6"/>
       <c r="S52" s="6"/>
       <c r="T52" s="6" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="U52" s="6"/>
       <c r="V52" s="6"/>
@@ -5520,7 +5514,7 @@
         <v>42</v>
       </c>
       <c r="AN52" s="9" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="AO52" s="6"/>
     </row>
@@ -5535,37 +5529,37 @@
         <v>42</v>
       </c>
       <c r="D53" s="6" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E53" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="F53" s="6" t="s">
         <v>236</v>
       </c>
-      <c r="F53" s="6" t="s">
+      <c r="G53" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="G53" s="6" t="s">
+      <c r="H53" s="6" t="s">
         <v>238</v>
-      </c>
-      <c r="H53" s="6" t="s">
-        <v>239</v>
       </c>
       <c r="I53" s="6"/>
       <c r="J53" s="6"/>
       <c r="K53" s="6" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="L53" s="6"/>
       <c r="M53" s="6"/>
       <c r="N53" s="6"/>
       <c r="O53" s="6"/>
       <c r="P53" s="7" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="Q53" s="6"/>
       <c r="R53" s="6"/>
       <c r="S53" s="6"/>
       <c r="T53" s="6" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="U53" s="6"/>
       <c r="V53" s="6"/>
@@ -5604,22 +5598,22 @@
         <v>42</v>
       </c>
       <c r="D54" s="6" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E54" s="6"/>
       <c r="F54" s="6" t="s">
+        <v>241</v>
+      </c>
+      <c r="G54" s="6" t="s">
         <v>242</v>
       </c>
-      <c r="G54" s="6" t="s">
-        <v>243</v>
-      </c>
       <c r="H54" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="I54" s="6"/>
       <c r="J54" s="6"/>
       <c r="K54" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="L54" s="6"/>
       <c r="M54" s="6"/>
@@ -5630,7 +5624,7 @@
       <c r="R54" s="6"/>
       <c r="S54" s="6"/>
       <c r="T54" s="6" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="U54" s="6"/>
       <c r="V54" s="6"/>

</xml_diff>